<commit_message>
Actualizacion de catalogos y de pestaña de comparacion
</commit_message>
<xml_diff>
--- a/catalogo/comparacion/datos_anteriores.xlsx
+++ b/catalogo/comparacion/datos_anteriores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -39,70 +39,14 @@
   <si>
     <t xml:space="preserve">X5</t>
   </si>
-  <si>
-    <t xml:space="preserve">2012-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-07</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -185,7 +129,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,6 +139,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,10 +166,13 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A20"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.17"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -244,382 +195,382 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="n">
+      <c r="A2" s="3" t="n">
+        <v>40909</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>100.382178252674</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="0" t="n">
         <v>0.062270434532</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="0" t="n">
         <v>100.732418225595</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="0" t="n">
         <v>0.071066395447</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="0" t="n">
         <v>100.883228629794</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="n">
+      <c r="A3" s="3" t="n">
+        <v>40940</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>100.422898454227</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="0" t="n">
         <v>0.040720201553</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="0" t="n">
         <v>100.780319842711</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="0" t="n">
         <v>0.047901617116</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="0" t="n">
         <v>100.948181413905</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="n">
+      <c r="A4" s="3" t="n">
+        <v>40969</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>100.447081321682</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="0" t="n">
         <v>0.024182867455</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="0" t="n">
         <v>100.801707187934</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="0" t="n">
         <v>0.021387345223</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="0" t="n">
         <v>100.981873708584</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="n">
+      <c r="A5" s="3" t="n">
+        <v>41000</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>100.456848232301</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="0" t="n">
         <v>0.009766910619</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="0" t="n">
         <v>100.799193889778</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="0" t="n">
         <v>-0.002513298156</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="0" t="n">
         <v>100.992868300711</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="n">
+      <c r="A6" s="3" t="n">
+        <v>41030</v>
+      </c>
+      <c r="B6" s="0" t="n">
         <v>100.452357846568</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="0" t="n">
         <v>-0.004490385733</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="0" t="n">
         <v>100.778633098968</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="0" t="n">
         <v>-0.020560790811</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="0" t="n">
         <v>100.983871703869</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="n">
+      <c r="A7" s="3" t="n">
+        <v>41061</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>100.441044438861</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="0" t="n">
         <v>-0.011313407707</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="0" t="n">
         <v>100.753735230439</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="0" t="n">
         <v>-0.024897868529</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="0" t="n">
         <v>100.954782406015</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="n">
+      <c r="A8" s="3" t="n">
+        <v>41091</v>
+      </c>
+      <c r="B8" s="0" t="n">
         <v>100.420168114064</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="0" t="n">
         <v>-0.020876324797</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="0" t="n">
         <v>100.720261868443</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <v>-0.033473361996</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="0" t="n">
         <v>100.891951642193</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="n">
+      <c r="A9" s="3" t="n">
+        <v>41122</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>100.387594560347</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="0" t="n">
         <v>-0.032573553718</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="0" t="n">
         <v>100.676809648549</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="0" t="n">
         <v>-0.043452219894</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="0" t="n">
         <v>100.784932532513</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="n">
+      <c r="A10" s="3" t="n">
+        <v>41153</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>100.346550488258</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="0" t="n">
         <v>-0.041044072089</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="0" t="n">
         <v>100.633708022172</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
         <v>-0.043101626377</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="0" t="n">
         <v>100.652525839786</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="n">
+      <c r="A11" s="3" t="n">
+        <v>41183</v>
+      </c>
+      <c r="B11" s="0" t="n">
         <v>100.289478388858</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="0" t="n">
         <v>-0.0570720994</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="0" t="n">
         <v>100.588371257614</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="0" t="n">
         <v>-0.045336764558</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="0" t="n">
         <v>100.496759771078</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="n">
+      <c r="A12" s="3" t="n">
+        <v>41214</v>
+      </c>
+      <c r="B12" s="0" t="n">
         <v>100.224795060421</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="0" t="n">
         <v>-0.064683328437</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="0" t="n">
         <v>100.534732935546</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="0" t="n">
         <v>-0.053638322068</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="0" t="n">
         <v>100.354562674954</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="n">
+      <c r="A13" s="3" t="n">
+        <v>41244</v>
+      </c>
+      <c r="B13" s="0" t="n">
         <v>100.158544268654</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="0" t="n">
         <v>-0.066250791766</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="0" t="n">
         <v>100.455925018339</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="0" t="n">
         <v>-0.078807917207</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="0" t="n">
         <v>100.22014712148</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="n">
+      <c r="A14" s="3" t="n">
+        <v>41275</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <v>100.099976341187</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="0" t="n">
         <v>-0.058567927468</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="0" t="n">
         <v>100.355321145558</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="0" t="n">
         <v>-0.100603872781</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="0" t="n">
         <v>100.093564341942</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2" t="n">
+      <c r="A15" s="3" t="n">
+        <v>41306</v>
+      </c>
+      <c r="B15" s="0" t="n">
         <v>100.046379551492</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="0" t="n">
         <v>-0.053596789695</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="0" t="n">
         <v>100.242555242783</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="0" t="n">
         <v>-0.112765902775</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="0" t="n">
         <v>99.967251565359</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2" t="n">
+      <c r="A16" s="3" t="n">
+        <v>41334</v>
+      </c>
+      <c r="B16" s="0" t="n">
         <v>99.991894917522</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="0" t="n">
         <v>-0.05448463397</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="0" t="n">
         <v>100.132453892174</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="0" t="n">
         <v>-0.110101350609</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="0" t="n">
         <v>99.831406835007</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2" t="n">
+      <c r="A17" s="3" t="n">
+        <v>41365</v>
+      </c>
+      <c r="B17" s="0" t="n">
         <v>99.94229993191</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="0" t="n">
         <v>-0.049594985612</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="0" t="n">
         <v>100.037086776441</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="0" t="n">
         <v>-0.095367115733</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="0" t="n">
         <v>99.711653248679</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="n">
+      <c r="A18" s="3" t="n">
+        <v>41395</v>
+      </c>
+      <c r="B18" s="0" t="n">
         <v>99.906545985231</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="0" t="n">
         <v>-0.035753946679</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="0" t="n">
         <v>99.964675966876</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="0" t="n">
         <v>-0.072410809565</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="0" t="n">
         <v>99.632684280093</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="2" t="n">
+      <c r="A19" s="3" t="n">
+        <v>41426</v>
+      </c>
+      <c r="B19" s="0" t="n">
         <v>99.870862203581</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="0" t="n">
         <v>-0.03568378165</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="0" t="n">
         <v>99.905320296737</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="0" t="n">
         <v>-0.059355670139</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="0" t="n">
         <v>99.573224639258</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="2" t="n">
+      <c r="A20" s="3" t="n">
+        <v>41456</v>
+      </c>
+      <c r="B20" s="0" t="n">
         <v>99.835466892018</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="0" t="n">
         <v>-0.035395311562</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="0" t="n">
         <v>99.860966880751</v>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="0" t="n">
         <v>-0.044353415986</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="0" t="n">
         <v>99.539183203497</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizando ejemplos y texto de vistas
</commit_message>
<xml_diff>
--- a/catalogo/comparacion/datos_anteriores.xlsx
+++ b/catalogo/comparacion/datos_anteriores.xlsx
@@ -165,8 +165,8 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,9 +321,6 @@
       <c r="B8" s="0" t="n">
         <v>100.420168114064</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>-0.020876324797</v>
-      </c>
       <c r="D8" s="0" t="n">
         <v>100.720261868443</v>
       </c>
@@ -341,9 +338,6 @@
       <c r="B9" s="0" t="n">
         <v>100.387594560347</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>-0.032573553718</v>
-      </c>
       <c r="D9" s="0" t="n">
         <v>100.676809648549</v>
       </c>
@@ -361,14 +355,8 @@
       <c r="B10" s="0" t="n">
         <v>100.346550488258</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>-0.041044072089</v>
-      </c>
       <c r="D10" s="0" t="n">
         <v>100.633708022172</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>-0.043101626377</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>100.652525839786</v>
@@ -407,9 +395,6 @@
       <c r="D12" s="0" t="n">
         <v>100.534732935546</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <v>-0.053638322068</v>
-      </c>
       <c r="F12" s="0" t="n">
         <v>100.354562674954</v>
       </c>
@@ -427,9 +412,6 @@
       <c r="D13" s="0" t="n">
         <v>100.455925018339</v>
       </c>
-      <c r="E13" s="0" t="n">
-        <v>-0.078807917207</v>
-      </c>
       <c r="F13" s="0" t="n">
         <v>100.22014712148</v>
       </c>
@@ -446,9 +428,6 @@
       </c>
       <c r="D14" s="0" t="n">
         <v>100.355321145558</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>-0.100603872781</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>100.093564341942</v>

</xml_diff>